<commit_message>
the website launch test script with test documents
</commit_message>
<xml_diff>
--- a/Daily action item list.xlsx
+++ b/Daily action item list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>30min.</t>
+  </si>
+  <si>
+    <t>45min</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,17 +101,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -409,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,56 +451,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>43480</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43480</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>43480</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>43480</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some sdditional codes on submita free ad link
</commit_message>
<xml_diff>
--- a/Daily action item list.xlsx
+++ b/Daily action item list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>link the local project with git</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <t>basic smoke test</t>
   </si>
 </sst>
 </file>
@@ -434,7 +446,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,33 +522,53 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43480</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>43480</v>
+        <v>43481</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -544,13 +576,17 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>43480</v>
+        <v>43481</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>

</xml_diff>